<commit_message>
remove long double and check for possible overflow, compare zero init vector and push_back (results.xlsx)
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -11,15 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>Window size measurements</t>
+    <t>Type measurements (push_back)</t>
   </si>
   <si>
-    <t>Window size measurements (float)</t>
-  </si>
-  <si>
-    <t>Type measurements</t>
+    <t>Type measurements (zeroes init)</t>
   </si>
   <si>
     <t>double</t>
@@ -98,7 +95,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t> относительно параметра "Window size measurements"</a:t>
+              <a:t>push_back</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -107,81 +104,48 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
+      <c:barChart>
+        <c:barDir val="col"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>results!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln>
-              <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:cat>
+            <c:strRef>
+              <c:f>results!$A$2:$A$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>results!$A$2:$A$7</c:f>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>results!$B$2:$B$7</c:f>
+              <c:f>results!$B$2:$B$3</c:f>
               <c:numCache/>
             </c:numRef>
-          </c:yVal>
+          </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="753288978"/>
-        <c:axId val="2030723853"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="753288978"/>
+        <c:axId val="1932695220"/>
+        <c:axId val="731394563"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1932695220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -203,7 +167,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Window size</a:t>
+                  <a:t/>
                 </a:r>
               </a:p>
             </c:rich>
@@ -213,10 +177,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
+        <c:spPr/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -231,13 +192,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2030723853"/>
-      </c:valAx>
+        <c:crossAx val="731394563"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="2030723853"/>
+        <c:axId val="731394563"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="3.0E7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -310,7 +270,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="753288978"/>
+        <c:crossAx val="1932695220"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -360,7 +320,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t> относительно параметра "Window size measurements float"</a:t>
+              <a:t>Zeroes init</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -369,81 +329,48 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
+      <c:barChart>
+        <c:barDir val="col"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>results!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln>
-              <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:cat>
+            <c:strRef>
+              <c:f>results!$C$2:$C$3</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>results!$A$9:$A$14</c:f>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>results!$B$9:$B$14</c:f>
+              <c:f>results!$D$2:$D$3</c:f>
               <c:numCache/>
             </c:numRef>
-          </c:yVal>
+          </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1353273098"/>
-        <c:axId val="1330122757"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1353273098"/>
+        <c:axId val="1065412439"/>
+        <c:axId val="1639706057"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1065412439"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -465,20 +392,25 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Window size</a:t>
+                  <a:t/>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.10486197916666666"/>
+              <c:y val="0.9149595687331536"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
+        <c:spPr/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -493,13 +425,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1330122757"/>
-      </c:valAx>
+        <c:crossAx val="1639706057"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="1330122757"/>
+        <c:axId val="1639706057"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="3.0E7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -572,269 +503,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1353273098"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t> относительно параметра "Type measurements"</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln cmpd="sng">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>results!$A$16:$A$17</c:f>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>results!$B$16:$B$17</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1617495631"/>
-        <c:axId val="2006904700"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1617495631"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>Type</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2006904700"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2006904700"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="3.0E7"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1617495631"/>
+        <c:crossAx val="1065412439"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -864,10 +533,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -889,10 +558,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -907,31 +576,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Диаграмма"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1148,130 +792,43 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>4.0</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>3.278237E7</v>
+        <v>1.2445086E8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.75318641E8</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
-        <v>8.0</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>3.3998803E7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3.4113858E7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3.3543877E7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>64.0</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3.4643912E7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <v>128.0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3.3827553E7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3.5938128E7</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3.639222E7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3.6652995E7</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="B12" s="1">
-        <v>3.6857934E7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1">
-        <v>64.0</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3.712931E7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1">
-        <v>128.0</v>
-      </c>
-      <c r="B14" s="1">
-        <v>3.726671E7</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
+        <v>1.63915616E8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="1">
-        <v>3.3998803E7</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3.5002117E7</v>
+      <c r="D3" s="1">
+        <v>1.99616735E8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>